<commit_message>
Standardize protein nomenclature: BBS and IFT naming
Database updates:
- BBIP1 → BBS18 (A8MTZ0)
- LZTFL1 → BBS17 (Q9NQ48)
- WDR19 → IFT144 (Q8NEZ3)
- WDR35 → IFT121 (Q9P2L0)

Supplementary data regenerated with standardized names.

Impact: All BBSome proteins now use BBS## naming, all IFT proteins use IFT### naming.
Improves sorting and consistency in dropdown menus and publications.

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Supplementary_Data_File_1_Complete_Dataset.xlsx
+++ b/Supplementary_Data_File_1_Complete_Dataset.xlsx
@@ -1024,7 +1024,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="E4" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="F4" t="str">
         <v>Homo sapiens</v>
@@ -1065,7 +1065,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B5" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C5" t="str">
         <v>Homo sapiens</v>
@@ -1415,7 +1415,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B12" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C12" t="str">
         <v>Homo sapiens</v>
@@ -1474,7 +1474,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="E13" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="F13" t="str">
         <v>Homo sapiens</v>
@@ -1874,7 +1874,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="E21" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="F21" t="str">
         <v>Homo sapiens</v>
@@ -2224,7 +2224,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="E28" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="F28" t="str">
         <v>Homo sapiens</v>
@@ -2315,7 +2315,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="B30" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C30" t="str">
         <v>Homo sapiens</v>
@@ -2574,7 +2574,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="E35" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="F35" t="str">
         <v>Homo sapiens</v>
@@ -2615,7 +2615,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="B36" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C36" t="str">
         <v>Homo sapiens</v>
@@ -2765,7 +2765,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B39" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C39" t="str">
         <v>Homo sapiens</v>
@@ -3174,7 +3174,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="E47" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="F47" t="str">
         <v>Homo sapiens</v>
@@ -3415,7 +3415,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B52" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C52" t="str">
         <v>Homo sapiens</v>
@@ -3665,7 +3665,7 @@
         <v>Q9NQ48</v>
       </c>
       <c r="B57" t="str">
-        <v>LZTFL1</v>
+        <v>BBS17</v>
       </c>
       <c r="C57" t="str">
         <v>Homo sapiens</v>
@@ -3674,7 +3674,7 @@
         <v>Q9NQ48</v>
       </c>
       <c r="E57" t="str">
-        <v>LZTFL1</v>
+        <v>BBS17</v>
       </c>
       <c r="F57" t="str">
         <v>Homo sapiens</v>
@@ -3865,7 +3865,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="B61" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C61" t="str">
         <v>Homo sapiens</v>
@@ -3974,7 +3974,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="E63" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="F63" t="str">
         <v>Homo sapiens</v>
@@ -4174,7 +4174,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="E67" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="F67" t="str">
         <v>Homo sapiens</v>
@@ -4265,7 +4265,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B69" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C69" t="str">
         <v>Homo sapiens</v>
@@ -6215,7 +6215,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B108" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C108" t="str">
         <v>Homo sapiens</v>
@@ -7415,7 +7415,7 @@
         <v>Q9NQ48</v>
       </c>
       <c r="B132" t="str">
-        <v>LZTFL1</v>
+        <v>BBS17</v>
       </c>
       <c r="C132" t="str">
         <v>Homo sapiens</v>
@@ -8115,7 +8115,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B146" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C146" t="str">
         <v>Homo sapiens</v>
@@ -8615,7 +8615,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B156" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C156" t="str">
         <v>Homo sapiens</v>
@@ -9865,7 +9865,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B181" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C181" t="str">
         <v>Homo sapiens</v>
@@ -10915,7 +10915,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B202" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C202" t="str">
         <v>Homo sapiens</v>
@@ -12515,7 +12515,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B234" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C234" t="str">
         <v>Homo sapiens</v>
@@ -14265,7 +14265,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B269" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C269" t="str">
         <v>Homo sapiens</v>
@@ -15565,7 +15565,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B295" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C295" t="str">
         <v>Homo sapiens</v>
@@ -15915,7 +15915,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B302" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C302" t="str">
         <v>Homo sapiens</v>
@@ -18962,7 +18962,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B363" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C363" t="str">
         <v>Homo sapiens</v>
@@ -20012,7 +20012,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B384" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C384" t="str">
         <v>Homo sapiens</v>
@@ -20712,7 +20712,7 @@
         <v>Q8NEZ3</v>
       </c>
       <c r="B398" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C398" t="str">
         <v>Homo sapiens</v>
@@ -21612,7 +21612,7 @@
         <v>Q9NQ48</v>
       </c>
       <c r="B416" t="str">
-        <v>LZTFL1</v>
+        <v>BBS17</v>
       </c>
       <c r="C416" t="str">
         <v>Homo sapiens</v>
@@ -21662,7 +21662,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B417" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C417" t="str">
         <v>Homo sapiens</v>
@@ -22762,7 +22762,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B439" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C439" t="str">
         <v>Homo sapiens</v>
@@ -23712,7 +23712,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B458" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C458" t="str">
         <v>Homo sapiens</v>
@@ -24012,7 +24012,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B464" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C464" t="str">
         <v>Homo sapiens</v>
@@ -24962,7 +24962,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B483" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C483" t="str">
         <v>Homo sapiens</v>
@@ -25612,7 +25612,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B496" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C496" t="str">
         <v>Homo sapiens</v>
@@ -26012,7 +26012,7 @@
         <v>Q9P2L0</v>
       </c>
       <c r="B504" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C504" t="str">
         <v>Homo sapiens</v>
@@ -28625,7 +28625,7 @@
         <v>A8MTZ0</v>
       </c>
       <c r="B14" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C14" t="str">
         <v>Homo sapiens</v>
@@ -28875,10 +28875,10 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>Q9Y366</v>
+        <v>Q9P2L0</v>
       </c>
       <c r="B25" t="str">
-        <v>IFT52</v>
+        <v>IFT121</v>
       </c>
       <c r="C25" t="str">
         <v>Homo sapiens</v>
@@ -28890,7 +28890,7 @@
         <v>9</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G25">
         <v>9</v>
@@ -28898,10 +28898,10 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Q9P2L0</v>
+        <v>Q9Y366</v>
       </c>
       <c r="B26" t="str">
-        <v>WDR35</v>
+        <v>IFT52</v>
       </c>
       <c r="C26" t="str">
         <v>Homo sapiens</v>
@@ -28913,7 +28913,7 @@
         <v>9</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G26">
         <v>9</v>
@@ -29128,10 +29128,10 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>Q9UG01</v>
+        <v>Q8NEZ3</v>
       </c>
       <c r="B36" t="str">
-        <v>IFT172</v>
+        <v>IFT144</v>
       </c>
       <c r="C36" t="str">
         <v>Homo sapiens</v>
@@ -29143,7 +29143,7 @@
         <v>4</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G36">
         <v>4</v>
@@ -29151,10 +29151,10 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>Q6UW49</v>
+        <v>Q9UG01</v>
       </c>
       <c r="B37" t="str">
-        <v>SPESP1</v>
+        <v>IFT172</v>
       </c>
       <c r="C37" t="str">
         <v>Homo sapiens</v>
@@ -29163,10 +29163,10 @@
         <v>Hs</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37">
         <v>4</v>
@@ -29174,10 +29174,10 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>Q96LJ8</v>
+        <v>Q6UW49</v>
       </c>
       <c r="B38" t="str">
-        <v>UBXN10</v>
+        <v>SPESP1</v>
       </c>
       <c r="C38" t="str">
         <v>Homo sapiens</v>
@@ -29197,10 +29197,10 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>Q8NEZ3</v>
+        <v>Q96LJ8</v>
       </c>
       <c r="B39" t="str">
-        <v>WDR19</v>
+        <v>UBXN10</v>
       </c>
       <c r="C39" t="str">
         <v>Homo sapiens</v>
@@ -29209,10 +29209,10 @@
         <v>Hs</v>
       </c>
       <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
         <v>4</v>
-      </c>
-      <c r="F39">
-        <v>3</v>
       </c>
       <c r="G39">
         <v>4</v>
@@ -29243,10 +29243,10 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Q9Y6A4</v>
+        <v>Q9NQ48</v>
       </c>
       <c r="B41" t="str">
-        <v>CFAP20</v>
+        <v>BBS17</v>
       </c>
       <c r="C41" t="str">
         <v>Homo sapiens</v>
@@ -29255,10 +29255,10 @@
         <v>Hs</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F41">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>3</v>
@@ -29266,10 +29266,10 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>Q717R9</v>
+        <v>Q9Y6A4</v>
       </c>
       <c r="B42" t="str">
-        <v>CYS1</v>
+        <v>CFAP20</v>
       </c>
       <c r="C42" t="str">
         <v>Homo sapiens</v>
@@ -29289,10 +29289,10 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>Q9UK59</v>
+        <v>Q717R9</v>
       </c>
       <c r="B43" t="str">
-        <v>DBR1</v>
+        <v>CYS1</v>
       </c>
       <c r="C43" t="str">
         <v>Homo sapiens</v>
@@ -29312,10 +29312,10 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>O75937</v>
+        <v>Q9UK59</v>
       </c>
       <c r="B44" t="str">
-        <v>DNAJC8</v>
+        <v>DBR1</v>
       </c>
       <c r="C44" t="str">
         <v>Homo sapiens</v>
@@ -29335,10 +29335,10 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>O95467</v>
+        <v>O75937</v>
       </c>
       <c r="B45" t="str">
-        <v>GNAS</v>
+        <v>DNAJC8</v>
       </c>
       <c r="C45" t="str">
         <v>Homo sapiens</v>
@@ -29358,10 +29358,10 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>P54257</v>
+        <v>O95467</v>
       </c>
       <c r="B46" t="str">
-        <v>HAP1</v>
+        <v>GNAS</v>
       </c>
       <c r="C46" t="str">
         <v>Homo sapiens</v>
@@ -29381,10 +29381,10 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>Q8WYA0</v>
+        <v>P54257</v>
       </c>
       <c r="B47" t="str">
-        <v>IFT81</v>
+        <v>HAP1</v>
       </c>
       <c r="C47" t="str">
         <v>Homo sapiens</v>
@@ -29393,10 +29393,10 @@
         <v>Hs</v>
       </c>
       <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>3</v>
-      </c>
-      <c r="F47">
-        <v>1</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -29404,10 +29404,10 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>Q9NQ48</v>
+        <v>Q8WYA0</v>
       </c>
       <c r="B48" t="str">
-        <v>LZTFL1</v>
+        <v>IFT81</v>
       </c>
       <c r="C48" t="str">
         <v>Homo sapiens</v>
@@ -44960,7 +44960,7 @@
         <v>BBS8</v>
       </c>
       <c r="B4" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C4">
         <v>0.7713359</v>
@@ -44980,7 +44980,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="B5" t="str">
         <v>BBS8</v>
@@ -45118,7 +45118,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="B11" t="str">
         <v>BBS4</v>
@@ -45144,7 +45144,7 @@
         <v>BBS4</v>
       </c>
       <c r="B12" t="str">
-        <v>BBIP1</v>
+        <v>BBS18</v>
       </c>
       <c r="C12">
         <v>0.7131941</v>
@@ -45351,7 +45351,7 @@
         <v>IFT122</v>
       </c>
       <c r="B21" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C21">
         <v>0.6876721</v>
@@ -45394,7 +45394,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="B23" t="str">
         <v>IFT122</v>
@@ -45581,7 +45581,7 @@
         <v>IFT122</v>
       </c>
       <c r="B31" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C31">
         <v>0.6582769</v>
@@ -45670,7 +45670,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="B35" t="str">
         <v>IFT122</v>
@@ -45716,7 +45716,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="B37" t="str">
         <v>IFT140</v>
@@ -45742,7 +45742,7 @@
         <v>IFT140</v>
       </c>
       <c r="B38" t="str">
-        <v>WDR19</v>
+        <v>IFT144</v>
       </c>
       <c r="C38">
         <v>0.6170063</v>
@@ -45811,7 +45811,7 @@
         <v>IFT43</v>
       </c>
       <c r="B41" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="C41">
         <v>0.5973592</v>
@@ -45831,7 +45831,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>WDR35</v>
+        <v>IFT121</v>
       </c>
       <c r="B42" t="str">
         <v>IFT43</v>

</xml_diff>